<commit_message>
scrapping dollar amount and location from craiglists, fixed the bedroom data along with the square footage. Not bringing anything else for attributes along right now, but could easily, code is just commented out.
</commit_message>
<xml_diff>
--- a/ Results 2019-07-27.xlsx
+++ b/ Results 2019-07-27.xlsx
@@ -345,7 +345,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F68"/>
+  <dimension ref="A1:H68"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -356,38 +356,140 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
+          <t>6943640752</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>https://minneapolis.craigslist.org/hnp/apa/d/eden-prairie-apartment-available-but/6943640752.html</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>$2024</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t> (Eden Prairie)</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>2BR / 2Ba</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>1119ft2</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>
+QR Code Link to This Post
+Transportation - The SW Metro transit station is less than two-miles away, so commuting downtown is a breeze. Shopping - Eden Prairie Center is less than a mile away with all the stores you will need. Dining - The Prairie Tap House, Wildfire, Redstone, Crave and many more wonderful eateries are just down the road. The Bluffs at Nine Mile Creek means affordable luxury, with every amenity you could want and convenience you have to experience to believe. Call and make an appointment to find your perfect home.  Community Amenities Include:  - In-Home Full-Size Washer &amp; Dryer  - Central Air-Conditioning  - Additional Parking Garage Space(s) Available To Rent  - Full-Demonstration Kitchen  - In-Home Fireplace  We are a pet friendly community! Dogs &amp; cats welcome!  *To maintain the integrity of the community, credit, criminal and rental background checks are conducted on all applicants. Office Hours: Monday-Thursday: 9:00AM-6:00PMFriday: 9:00AM-5:00PMSaturday: 10:00AM-4:00PMSunday:12:00PM-4:00PM  Call today to learn more about our community:  show contact info
+Bluffs At Nine Mile Creek 7475 Flying Cloud Drive Eden Prairie, MN, 55344  http://rent.dominiumapartments.com/73Lz53Equal Housing Opportunity *Some Restrictions May Apply.GCouig4BK4iW </t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>6938924680</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>https://minneapolis.craigslist.org/hnp/apa/d/eden-prairie-spacious-staring-staring/6938924680.html</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>$1691</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>None Found</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>2BR / 2Ba</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>1198ft2</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>
+QR Code Link to This Post
+Premier Eden Prairie Apartments Live luxuriously in the heart of Eden Prairie, MN! Arrive Watertower is a beautifully landscaped, modern community with upscale in-home features and a dizzying array of luxury community amenities.
+-In-Unit Laundry
+-Accepts Electronic Payments
+-Conference Room
+-Tile Floors
+-Old Chicago Restaurant On-site
+-Controlled Access
+-Cable Ready
+-Alarm System
+Call:  show contact info
+.
+Hot Tub/Sauna, State of the Art Upgrades, On-Site Management, Cabana Seating, Exquisite Design, Beautifully Remodeled , Al Fresco Dining in Courtyard, Close to Shopping, Electronic Payments, Luxurious, Groundskeeping, Wide Range of Floor Plans, Lighting Upgrades, 24 Hour Access, Basketball Court    </t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
           <t>6942985683</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="B3" t="inlineStr">
         <is>
           <t>6819253190</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>
-2BR / 2.5Ba
-1515ft2
-available jul 26
-</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>
-cats are OK - purrr
-dogs are OK - wooof
-townhouse
-w/d in unit
-no smoking
-attached garage
-wheelchair accessible
-</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr"/>
-      <c r="F1" t="inlineStr">
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>https://minneapolis.craigslist.org/dak/apa/d/saint-paul-renovated-spacious-2-bedroom/6942985683.html</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>$1690</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t> (Apple Valley)</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>2BR / 2.5Ba</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>1515ft2</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
         <is>
           <t>
 QR Code Link to This Post
@@ -427,40 +529,43 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
+    <row r="4">
+      <c r="A4" t="inlineStr">
         <is>
           <t>6937828893</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="B4" t="inlineStr">
         <is>
           <t>None</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>
-2BR / 2Ba
-1082ft2
-</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>
-cats are OK - purrr
-dogs are OK - wooof
-apartment
-w/d in unit
-no smoking
-attached garage
-wheelchair accessible
-</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr">
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>https://minneapolis.craigslist.org/hnp/apa/d/minneapolis-game-lounge-fire-pit-bike/6937828893.html</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>$2015</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>None Found</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>2BR / 2Ba</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>1082ft2</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
         <is>
           <t>
 QR Code Link to This Post
@@ -486,41 +591,43 @@
         </is>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
+    <row r="5">
+      <c r="A5" t="inlineStr">
         <is>
           <t>6929306647</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="B5" t="inlineStr">
         <is>
           <t>None</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>
-2BR / 2Ba
-1026ft2
-available aug 22
-</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>
-cats are OK - purrr
-dogs are OK - wooof
-apartment
-w/d in unit
-no smoking
-attached garage
-wheelchair accessible
-</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr">
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>https://minneapolis.craigslist.org/hnp/apa/d/minneapolis-amenities-galore-take-tour/6929306647.html</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>$2245</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t> (7161 France Avenue South Edina, MN 55435)</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>2BR / 2Ba</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>1026ft2</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
         <is>
           <t>
 QR Code Link to This Post
@@ -529,102 +636,6 @@
         </is>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>6942696400</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>
-2BR / 2Ba
-1119ft2
-</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>
-cats are OK - purrr
-dogs are OK - wooof
-furnished
-apartment
-w/d in unit
-no smoking
-attached garage
-wheelchair accessible
-</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>
-QR Code Link to This Post
-The Bluffs at Nine Mile Creek - Spacious luxury in Eden Prairie that includes not just everything you need, but everything you want as well. Located in Eden Prairie's Golden Triangle, you have easy access to freeways, public transportation and park and rides. Our beautiful community is just minutes away from terrific restaurants, great shopping and all the entertainment you could need. You will love living at the Bluffs at Nine Mile Creek. Visit us today to discover your new home!  Community Amenities Include:  - Ample Counter Top &amp; Cabinet Space  - Community Participates In A Water, Sewer &amp; Trash Conservation Program  - Stainless Steel Kitchen Appliances  - Raised Panel Doors &amp; 9-Foot Ceilings  - Luxury Granite Counter Tops! (Select Homes)  - Furnished Apartments Available  - Outdoor Off-Street Open Parking Available  - Full-Demonstration Kitchen  We are a pet friendly community! Dogs &amp; cats welcome!  *To maintain the integrity of the community, credit, criminal and rental background checks are conducted on all applicants. Office Hours: Monday-Thursday: 9:00AM-6:00PMFriday: 9:00AM-5:00PMSaturday: 10:00AM-4:00PMSunday:12:00PM-4:00PM  Make the move today by giving our professional staff a call:  show contact info
-Bluffs At Nine Mile Creek 7475 Flying Cloud Drive Eden Prairie, MN, 55344  http://rent.dominiumapartments.com/rhLy46Equal Housing Opportunity *Some Restrictions May Apply.WCrpp5XP </t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>6938924680</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>
-2BR / 2Ba
-1198ft2
-available sep 11
-</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>
-cats are OK - purrr
-dogs are OK - wooof
-apartment
-w/d in unit
-no smoking
-attached garage
-wheelchair accessible
-</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr"/>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>
-QR Code Link to This Post
-Premier Eden Prairie Apartments Live luxuriously in the heart of Eden Prairie, MN! Arrive Watertower is a beautifully landscaped, modern community with upscale in-home features and a dizzying array of luxury community amenities.
--In-Unit Laundry
--Accepts Electronic Payments
--Conference Room
--Tile Floors
--Old Chicago Restaurant On-site
--Controlled Access
--Cable Ready
--Alarm System
-Call:  show contact info
-.
-Hot Tub/Sauna, State of the Art Upgrades, On-Site Management, Cabana Seating, Exquisite Design, Beautifully Remodeled , Al Fresco Dining in Courtyard, Close to Shopping, Electronic Payments, Luxurious, Groundskeeping, Wide Range of Floor Plans, Lighting Upgrades, 24 Hour Access, Basketball Court    </t>
-        </is>
-      </c>
-    </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
@@ -638,36 +649,30 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>
-2BR / 2Ba
-1455ft2
-available sep 11
-</t>
+          <t>https://minneapolis.craigslist.org/hnp/apa/d/eden-prairie-modern-community-luxury/6941915584.html</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>
-open house dates
-friday 2019-07-26
-saturday 2019-07-27
-</t>
+          <t>$1691</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>
-cats are OK - purrr
-dogs are OK - wooof
-apartment
-w/d in unit
-no smoking
-attached garage
-wheelchair accessible
-</t>
+          <t>None Found</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
+        <is>
+          <t>2BR / 2Ba</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>1455ft2</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
         <is>
           <t>
 QR Code Link to This Post
@@ -699,27 +704,30 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>
-2BR / 2Ba
-1218ft2
-</t>
+          <t>https://minneapolis.craigslist.org/hnp/apa/d/minneapolis-fitness-center-business/6931699662.html</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>
-cats are OK - purrr
-dogs are OK - wooof
-apartment
-w/d in unit
-no smoking
-attached garage
-wheelchair accessible
-</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr"/>
+          <t>$2260</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>None Found</t>
+        </is>
+      </c>
       <c r="F7" t="inlineStr">
+        <is>
+          <t>2BR / 2Ba</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>1218ft2</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
         <is>
           <t>
 QR Code Link to This Post
@@ -758,28 +766,30 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>
-3BR / 2Ba
-1486ft2
-available aug 6
-</t>
+          <t>https://minneapolis.craigslist.org/dak/apa/d/burnsville-unique-and-beautiful-3-bed/6941188895.html</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>
-cats are OK - purrr
-dogs are OK - wooof
-apartment
-w/d in unit
-no smoking
-attached garage
-wheelchair accessible
-</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr"/>
+          <t>$1811</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t> (Lakeville)</t>
+        </is>
+      </c>
       <c r="F8" t="inlineStr">
+        <is>
+          <t>3BR / 2Ba</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>1486ft2</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
         <is>
           <t>
 QR Code Link to This Post
@@ -814,27 +824,30 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>
-2BR / 2Ba
-1082ft2
-</t>
+          <t>https://minneapolis.craigslist.org/hnp/apa/d/minneapolis-private-balcony-package/6937694000.html</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>
-cats are OK - purrr
-dogs are OK - wooof
-apartment
-w/d in unit
-no smoking
-attached garage
-wheelchair accessible
-</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr"/>
+          <t>$2015</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>None Found</t>
+        </is>
+      </c>
       <c r="F9" t="inlineStr">
+        <is>
+          <t>2BR / 2Ba</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>1082ft2</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
         <is>
           <t>
 QR Code Link to This Post
@@ -873,27 +886,30 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>
-2BR / 2Ba
-975ft2
-</t>
+          <t>https://minneapolis.craigslist.org/hnp/apa/d/minneapolis-location-community-quality/6932255139.html</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>
-cats are OK - purrr
-dogs are OK - wooof
-apartment
-w/d in unit
-no smoking
-attached garage
-wheelchair accessible
-</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr"/>
+          <t>$2270</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t> (7161 France Avenue South Edina, MN 55435)</t>
+        </is>
+      </c>
       <c r="F10" t="inlineStr">
+        <is>
+          <t>2BR / 2Ba</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>975ft2</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
         <is>
           <t>
 QR Code Link to This Post
@@ -915,27 +931,30 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>
-2BR / 2Ba
-1033ft2
-</t>
+          <t>https://minneapolis.craigslist.org/hnp/apa/d/minneapolis-luxury-all-around/6932342750.html</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>
-cats are OK - purrr
-dogs are OK - wooof
-apartment
-w/d in unit
-no smoking
-attached garage
-wheelchair accessible
-</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr"/>
+          <t>$2360</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t> (7161 France Avenue South Edina, MN 55435)</t>
+        </is>
+      </c>
       <c r="F11" t="inlineStr">
+        <is>
+          <t>2BR / 2Ba</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>1033ft2</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
         <is>
           <t>
 QR Code Link to This Post
@@ -957,28 +976,30 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>
-2BR / 2.5Ba
-1515ft2
-available jul 22
-</t>
+          <t>https://minneapolis.craigslist.org/dak/apa/d/saint-paul-amazing-2-bedroom-townhome/6937627758.html</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>
-cats are OK - purrr
-dogs are OK - wooof
-townhouse
-w/d in unit
-no smoking
-attached garage
-wheelchair accessible
-</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr"/>
+          <t>$1690</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t> (Apple Valley)</t>
+        </is>
+      </c>
       <c r="F12" t="inlineStr">
+        <is>
+          <t>2BR / 2.5Ba</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>1515ft2</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
         <is>
           <t>
 QR Code Link to This Post
@@ -1030,28 +1051,30 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>
-2BR / 2.5Ba
-1515ft2
-available jul 21
-</t>
+          <t>https://minneapolis.craigslist.org/dak/apa/d/saint-paul-amazing-2-bedroom-townhome/6939064656.html</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>
-cats are OK - purrr
-dogs are OK - wooof
-townhouse
-w/d in unit
-no smoking
-attached garage
-wheelchair accessible
-</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr"/>
+          <t>$1690</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t> (Apple Valley)</t>
+        </is>
+      </c>
       <c r="F13" t="inlineStr">
+        <is>
+          <t>2BR / 2.5Ba</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>1515ft2</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
         <is>
           <t>
 QR Code Link to This Post
@@ -1103,27 +1126,30 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>
-2BR / 2Ba
-1033ft2
-</t>
+          <t>https://minneapolis.craigslist.org/hnp/apa/d/minneapolis-home-for-you-your-furry/6929081230.html</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>
-cats are OK - purrr
-dogs are OK - wooof
-apartment
-w/d in unit
-no smoking
-attached garage
-wheelchair accessible
-</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr"/>
+          <t>$2390</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t> (7161 France Avenue South Edina, MN 55435)</t>
+        </is>
+      </c>
       <c r="F14" t="inlineStr">
+        <is>
+          <t>2BR / 2Ba</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>1033ft2</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
         <is>
           <t>
 QR Code Link to This Post
@@ -1145,27 +1171,30 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>
-2BR / 2Ba
-1218ft2
-</t>
+          <t>https://minneapolis.craigslist.org/hnp/apa/d/minneapolis-fire-pit-close-to-freeway/6922378454.html</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>
-cats are OK - purrr
-dogs are OK - wooof
-apartment
-w/d in unit
-no smoking
-attached garage
-wheelchair accessible
-</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr"/>
+          <t>$2260</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>None Found</t>
+        </is>
+      </c>
       <c r="F15" t="inlineStr">
+        <is>
+          <t>2BR / 2Ba</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>1218ft2</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
         <is>
           <t>
 QR Code Link to This Post
@@ -1204,28 +1233,30 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>
-2BR / 2Ba
-1033ft2
-available jul 16
-</t>
+          <t>https://minneapolis.craigslist.org/hnp/apa/d/minneapolis-sit-back-relax-your-new/6935321981.html</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>
-cats are OK - purrr
-dogs are OK - wooof
-apartment
-w/d in unit
-no smoking
-attached garage
-wheelchair accessible
-</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr"/>
+          <t>$2370</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>None Found</t>
+        </is>
+      </c>
       <c r="F16" t="inlineStr">
+        <is>
+          <t>2BR / 2Ba</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>1033ft2</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
         <is>
           <t>
 QR Code Link to This Post
@@ -1271,27 +1302,30 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>
-2BR / 2Ba
-1455ft2
-</t>
+          <t>https://minneapolis.craigslist.org/hnp/apa/d/eden-prairie-spacious-2-bed-2-bath-only/6936684928.html</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>
-cats are OK - purrr
-dogs are OK - wooof
-apartment
-w/d in unit
-no smoking
-attached garage
-wheelchair accessible
-</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr"/>
+          <t>$1691</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>None Found</t>
+        </is>
+      </c>
       <c r="F17" t="inlineStr">
+        <is>
+          <t>2BR / 2Ba</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>1455ft2</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
         <is>
           <t>
 QR Code Link to This Post
@@ -1323,28 +1357,30 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>
-2BR / 2.5Ba
-1515ft2
-available jul 17
-</t>
+          <t>https://minneapolis.craigslist.org/dak/apa/d/saint-paul-amazing-2-bedroom-townhome/6936369678.html</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>
-cats are OK - purrr
-dogs are OK - wooof
-townhouse
-w/d in unit
-no smoking
-attached garage
-wheelchair accessible
-</t>
-        </is>
-      </c>
-      <c r="E18" t="inlineStr"/>
+          <t>$1640</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t> (Apple Valley)</t>
+        </is>
+      </c>
       <c r="F18" t="inlineStr">
+        <is>
+          <t>2BR / 2.5Ba</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>1515ft2</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
         <is>
           <t>
 QR Code Link to This Post
@@ -1397,28 +1433,30 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>
-3BR / 2Ba
-1486ft2
-available aug 8
-</t>
+          <t>https://minneapolis.craigslist.org/dak/apa/d/lakeville-hard-to-find-3-bd-2ba-corner/6935310024.html</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>
-cats are OK - purrr
-dogs are OK - wooof
-apartment
-w/d in unit
-no smoking
-attached garage
-wheelchair accessible
-</t>
-        </is>
-      </c>
-      <c r="E19" t="inlineStr"/>
+          <t>$1811</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t> (LAKEVILLE)</t>
+        </is>
+      </c>
       <c r="F19" t="inlineStr">
+        <is>
+          <t>3BR / 2Ba</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>1486ft2</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
         <is>
           <t>
 QR Code Link to This Post
@@ -1456,28 +1494,30 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>
-2BR / 2.5Ba
-1515ft2
-available aug 1
-</t>
+          <t>https://minneapolis.craigslist.org/dak/apa/d/saint-paul-amazing-2-bedroom-townhome/6935269311.html</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>
-cats are OK - purrr
-dogs are OK - wooof
-townhouse
-w/d in unit
-no smoking
-attached garage
-wheelchair accessible
-</t>
-        </is>
-      </c>
-      <c r="E20" t="inlineStr"/>
+          <t>$1715</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t> (Apple Valley)</t>
+        </is>
+      </c>
       <c r="F20" t="inlineStr">
+        <is>
+          <t>2BR / 2.5Ba</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>1515ft2</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
         <is>
           <t>
 QR Code Link to This Post
@@ -1529,28 +1569,30 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>
-2BR / 2.5Ba
-1515ft2
-available jul 16
-</t>
+          <t>https://minneapolis.craigslist.org/dak/apa/d/saint-paul-amazing-2-bedroom-townhome/6935250317.html</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>
-cats are OK - purrr
-dogs are OK - wooof
-townhouse
-w/d in unit
-no smoking
-attached garage
-wheelchair accessible
-</t>
-        </is>
-      </c>
-      <c r="E21" t="inlineStr"/>
+          <t>$1640</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t> (Apple Valley)</t>
+        </is>
+      </c>
       <c r="F21" t="inlineStr">
+        <is>
+          <t>2BR / 2.5Ba</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>1515ft2</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
         <is>
           <t>
 QR Code Link to This Post
@@ -1602,27 +1644,30 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>
-2BR / 2Ba
-1033ft2
-</t>
+          <t>https://minneapolis.craigslist.org/hnp/apa/d/minneapolis-experience-the-71-france/6915608103.html</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>
-cats are OK - purrr
-dogs are OK - wooof
-apartment
-w/d in unit
-no smoking
-attached garage
-wheelchair accessible
-</t>
-        </is>
-      </c>
-      <c r="E22" t="inlineStr"/>
+          <t>$2370</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t> (7161 France Avenue South Edina, MN 55435)</t>
+        </is>
+      </c>
       <c r="F22" t="inlineStr">
+        <is>
+          <t>2BR / 2Ba</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>1033ft2</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
         <is>
           <t>
 QR Code Link to This Post
@@ -1644,28 +1689,30 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>
-2BR / 2.5Ba
-1515ft2
-available jul 15
-</t>
+          <t>https://minneapolis.craigslist.org/dak/apa/d/saint-paul-amazing-2-bedroom-townhome/6934468965.html</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>
-cats are OK - purrr
-dogs are OK - wooof
-townhouse
-w/d in unit
-no smoking
-attached garage
-wheelchair accessible
-</t>
-        </is>
-      </c>
-      <c r="E23" t="inlineStr"/>
+          <t>$1715</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t> (Apple Valley)</t>
+        </is>
+      </c>
       <c r="F23" t="inlineStr">
+        <is>
+          <t>2BR / 2.5Ba</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>1515ft2</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
         <is>
           <t>
 QR Code Link to This Post
@@ -1717,28 +1764,30 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>
-2BR / 2Ba
-1080ft2
-available aug 6
-</t>
+          <t>https://minneapolis.craigslist.org/dak/apa/d/saint-paul-2-bedroom-available-starting/6933924134.html</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>
-cats are OK - purrr
-dogs are OK - wooof
-apartment
-w/d in unit
-no smoking
-attached garage
-wheelchair accessible
-</t>
-        </is>
-      </c>
-      <c r="E24" t="inlineStr"/>
+          <t>$1905</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t> (Apple Valley, MN)</t>
+        </is>
+      </c>
       <c r="F24" t="inlineStr">
+        <is>
+          <t>2BR / 2Ba</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>1080ft2</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
         <is>
           <t>
 QR Code Link to This Post
@@ -1762,28 +1811,30 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>
-2BR / 2.5Ba
-1515ft2
-available jul 13
-</t>
+          <t>https://minneapolis.craigslist.org/dak/apa/d/saint-paul-amazing-2-bedroom-townhome/6933158095.html</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>
-cats are OK - purrr
-dogs are OK - wooof
-townhouse
-w/d in unit
-no smoking
-attached garage
-wheelchair accessible
-</t>
-        </is>
-      </c>
-      <c r="E25" t="inlineStr"/>
+          <t>$1616</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t> (Apple Valley)</t>
+        </is>
+      </c>
       <c r="F25" t="inlineStr">
+        <is>
+          <t>2BR / 2.5Ba</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>1515ft2</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
         <is>
           <t>
 QR Code Link to This Post
@@ -1835,27 +1886,30 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>
-2BR / 2Ba
-1219ft2
-</t>
+          <t>https://minneapolis.craigslist.org/hnp/apa/d/minneapolis-yoga-spin-club-bike-storage/6930870713.html</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>
-cats are OK - purrr
-dogs are OK - wooof
-apartment
-w/d in unit
-no smoking
-attached garage
-wheelchair accessible
-</t>
-        </is>
-      </c>
-      <c r="E26" t="inlineStr"/>
+          <t>$2155</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>None Found</t>
+        </is>
+      </c>
       <c r="F26" t="inlineStr">
+        <is>
+          <t>2BR / 2Ba</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>1219ft2</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
         <is>
           <t>
 QR Code Link to This Post
@@ -1894,27 +1948,30 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>
-2BR / 2Ba
-1082ft2
-</t>
+          <t>https://minneapolis.craigslist.org/hnp/apa/d/minneapolis-custom-cabinetry-recycling/6925945288.html</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>
-cats are OK - purrr
-dogs are OK - wooof
-apartment
-w/d in unit
-no smoking
-attached garage
-wheelchair accessible
-</t>
-        </is>
-      </c>
-      <c r="E27" t="inlineStr"/>
+          <t>$2015</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>None Found</t>
+        </is>
+      </c>
       <c r="F27" t="inlineStr">
+        <is>
+          <t>2BR / 2Ba</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>1082ft2</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
         <is>
           <t>
 QR Code Link to This Post
@@ -1953,28 +2010,30 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>
-2BR / 2.5Ba
-1515ft2
-available aug 1
-</t>
+          <t>https://minneapolis.craigslist.org/dak/apa/d/saint-paul-amazing-2-bedroom-townhome/6931623072.html</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>
-cats are OK - purrr
-dogs are OK - wooof
-townhouse
-w/d in unit
-no smoking
-attached garage
-wheelchair accessible
-</t>
-        </is>
-      </c>
-      <c r="E28" t="inlineStr"/>
+          <t>$1691</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t> (Apple Valley)</t>
+        </is>
+      </c>
       <c r="F28" t="inlineStr">
+        <is>
+          <t>2BR / 2.5Ba</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>1515ft2</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
         <is>
           <t>
 QR Code Link to This Post
@@ -2026,27 +2085,30 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>
-2BR / 2Ba
-1193ft2
-</t>
+          <t>https://minneapolis.craigslist.org/hnp/apa/d/minneapolis-fire-sprinklers-bike-repair/6931543424.html</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>
-cats are OK - purrr
-dogs are OK - wooof
-apartment
-w/d in unit
-no smoking
-attached garage
-wheelchair accessible
-</t>
-        </is>
-      </c>
-      <c r="E29" t="inlineStr"/>
+          <t>$2110</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>None Found</t>
+        </is>
+      </c>
       <c r="F29" t="inlineStr">
+        <is>
+          <t>2BR / 2Ba</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>1193ft2</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
         <is>
           <t>
 QR Code Link to This Post
@@ -2085,28 +2147,30 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>
-3BR / 2Ba
-1475ft2
-available jul 11
-</t>
+          <t>https://minneapolis.craigslist.org/dak/apa/d/saint-paul-huge-3-bedroom-ready-for/6931506158.html</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>
-cats are OK - purrr
-dogs are OK - wooof
-apartment
-w/d in unit
-no smoking
-attached garage
-wheelchair accessible
-</t>
-        </is>
-      </c>
-      <c r="E30" t="inlineStr"/>
+          <t>$1947</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t> (Apple Valley)</t>
+        </is>
+      </c>
       <c r="F30" t="inlineStr">
+        <is>
+          <t>3BR / 2Ba</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>1475ft2</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr">
         <is>
           <t>
 QR Code Link to This Post
@@ -2154,28 +2218,30 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>
-2BR / 2.5Ba
-1515ft2
-available jul 11
-</t>
+          <t>https://minneapolis.craigslist.org/dak/apa/d/saint-paul-amazing-2-bedroom-townhome/6931502104.html</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>
-cats are OK - purrr
-dogs are OK - wooof
-townhouse
-w/d in unit
-no smoking
-attached garage
-wheelchair accessible
-</t>
-        </is>
-      </c>
-      <c r="E31" t="inlineStr"/>
+          <t>$1616</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t> (Apple Valley)</t>
+        </is>
+      </c>
       <c r="F31" t="inlineStr">
+        <is>
+          <t>2BR / 2.5Ba</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>1515ft2</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
         <is>
           <t>
 QR Code Link to This Post
@@ -2227,28 +2293,30 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>
-3BR / 2Ba
-1475ft2
-available jul 15
-</t>
+          <t>https://minneapolis.craigslist.org/dak/apa/d/saint-paul-huge-3-bedroom-ready-for/6930731147.html</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>
-cats are OK - purrr
-dogs are OK - wooof
-apartment
-w/d in unit
-no smoking
-attached garage
-wheelchair accessible
-</t>
-        </is>
-      </c>
-      <c r="E32" t="inlineStr"/>
+          <t>$2046</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t> (Apple Valley)</t>
+        </is>
+      </c>
       <c r="F32" t="inlineStr">
+        <is>
+          <t>3BR / 2Ba</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>1475ft2</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr">
         <is>
           <t>
 QR Code Link to This Post
@@ -2296,28 +2364,30 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>
-2BR / 2.5Ba
-1515ft2
-available jul 15
-</t>
+          <t>https://minneapolis.craigslist.org/dak/apa/d/saint-paul-amazing-2-bedroom-townhome/6930694708.html</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>
-cats are OK - purrr
-dogs are OK - wooof
-townhouse
-w/d in unit
-no smoking
-attached garage
-wheelchair accessible
-</t>
-        </is>
-      </c>
-      <c r="E33" t="inlineStr"/>
+          <t>$1715</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t> (Apple Valley)</t>
+        </is>
+      </c>
       <c r="F33" t="inlineStr">
+        <is>
+          <t>2BR / 2.5Ba</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>1515ft2</t>
+        </is>
+      </c>
+      <c r="H33" t="inlineStr">
         <is>
           <t>
 QR Code Link to This Post
@@ -2369,27 +2439,30 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>
-3BR / 2Ba
-1486ft2
-</t>
+          <t>https://minneapolis.craigslist.org/dak/apa/d/burnsville-spacious-beautiful-3-bed-2/6930155191.html</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>
-cats are OK - purrr
-dogs are OK - wooof
-apartment
-w/d in unit
-no smoking
-attached garage
-wheelchair accessible
-</t>
-        </is>
-      </c>
-      <c r="E34" t="inlineStr"/>
+          <t>$1811</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t> (Lakeville)</t>
+        </is>
+      </c>
       <c r="F34" t="inlineStr">
+        <is>
+          <t>3BR / 2Ba</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>1486ft2</t>
+        </is>
+      </c>
+      <c r="H34" t="inlineStr">
         <is>
           <t>
 QR Code Link to This Post
@@ -2423,28 +2496,30 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>
-3BR / 2Ba
-1475ft2
-available jul 9
-</t>
+          <t>https://minneapolis.craigslist.org/dak/apa/d/saint-paul-huge-3-bedroom-ready-for/6929922947.html</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>
-cats are OK - purrr
-dogs are OK - wooof
-apartment
-w/d in unit
-no smoking
-attached garage
-wheelchair accessible
-</t>
-        </is>
-      </c>
-      <c r="E35" t="inlineStr"/>
+          <t>$2046</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t> (Apple Valley)</t>
+        </is>
+      </c>
       <c r="F35" t="inlineStr">
+        <is>
+          <t>3BR / 2Ba</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>1475ft2</t>
+        </is>
+      </c>
+      <c r="H35" t="inlineStr">
         <is>
           <t>
 QR Code Link to This Post
@@ -2492,27 +2567,30 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>
-2BR / 2Ba
-975ft2
-</t>
+          <t>https://minneapolis.craigslist.org/hnp/apa/d/minneapolis-where-the-city-is-your/6927179366.html</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>
-cats are OK - purrr
-dogs are OK - wooof
-apartment
-w/d in unit
-no smoking
-attached garage
-wheelchair accessible
-</t>
-        </is>
-      </c>
-      <c r="E36" t="inlineStr"/>
+          <t>$2280</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t> (7161 France Avenue South Edina, MN 55435)</t>
+        </is>
+      </c>
       <c r="F36" t="inlineStr">
+        <is>
+          <t>2BR / 2Ba</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>975ft2</t>
+        </is>
+      </c>
+      <c r="H36" t="inlineStr">
         <is>
           <t>
 QR Code Link to This Post
@@ -2543,27 +2621,30 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>
-2BR / 2Ba
-1033ft2
-</t>
+          <t>https://minneapolis.craigslist.org/hnp/apa/d/minneapolis-apartments-tailored-to-your/6927267631.html</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>
-cats are OK - purrr
-dogs are OK - wooof
-apartment
-w/d in unit
-no smoking
-attached garage
-wheelchair accessible
-</t>
-        </is>
-      </c>
-      <c r="E37" t="inlineStr"/>
+          <t>$2360</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t> (7161 France Avenue South Edina, MN 55435)</t>
+        </is>
+      </c>
       <c r="F37" t="inlineStr">
+        <is>
+          <t>2BR / 2Ba</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>1033ft2</t>
+        </is>
+      </c>
+      <c r="H37" t="inlineStr">
         <is>
           <t>
 QR Code Link to This Post
@@ -2585,28 +2666,30 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>
-2BR / 2Ba
-968ft2
-available jul 20
-</t>
+          <t>https://minneapolis.craigslist.org/hnp/apa/d/minneapolis-the-lifestyle-you-deserve/6929179885.html</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>
-cats are OK - purrr
-dogs are OK - wooof
-apartment
-w/d in unit
-no smoking
-attached garage
-wheelchair accessible
-</t>
-        </is>
-      </c>
-      <c r="E38" t="inlineStr"/>
+          <t>$2265</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t> (7161 France Avenue South Edina, MN 55435)</t>
+        </is>
+      </c>
       <c r="F38" t="inlineStr">
+        <is>
+          <t>2BR / 2Ba</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>968ft2</t>
+        </is>
+      </c>
+      <c r="H38" t="inlineStr">
         <is>
           <t>
 QR Code Link to This Post
@@ -2637,28 +2720,30 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>
-3BR / 2Ba
-1475ft2
-available jul 5
-</t>
+          <t>https://minneapolis.craigslist.org/dak/apa/d/saint-paul-huge-3-bedroom-ready-for/6927123603.html</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>
-cats are OK - purrr
-dogs are OK - wooof
-apartment
-w/d in unit
-no smoking
-attached garage
-wheelchair accessible
-</t>
-        </is>
-      </c>
-      <c r="E39" t="inlineStr"/>
+          <t>$2046</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t> (Apple Valley)</t>
+        </is>
+      </c>
       <c r="F39" t="inlineStr">
+        <is>
+          <t>3BR / 2Ba</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>1475ft2</t>
+        </is>
+      </c>
+      <c r="H39" t="inlineStr">
         <is>
           <t>
 QR Code Link to This Post
@@ -2706,28 +2791,30 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>
-2BR / 2.5Ba
-1515ft2
-available jul 8
-</t>
+          <t>https://minneapolis.craigslist.org/dak/apa/d/saint-paul-amazing-2-bedroom-townhome/6927025374.html</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>
-cats are OK - purrr
-dogs are OK - wooof
-townhouse
-w/d in unit
-no smoking
-attached garage
-wheelchair accessible
-</t>
-        </is>
-      </c>
-      <c r="E40" t="inlineStr"/>
+          <t>$1777</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t> (Apple Valley)</t>
+        </is>
+      </c>
       <c r="F40" t="inlineStr">
+        <is>
+          <t>2BR / 2.5Ba</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>1515ft2</t>
+        </is>
+      </c>
+      <c r="H40" t="inlineStr">
         <is>
           <t>
 QR Code Link to This Post
@@ -2779,27 +2866,30 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>
-2BR / 2Ba
-1020ft2
-available jul 5
-</t>
+          <t>https://minneapolis.craigslist.org/hnp/apa/d/minneapolis-spacious-bloomington-2/6927024175.html</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>
-cats are OK - purrr
-apartment
-w/d in unit
-no smoking
-attached garage
-wheelchair accessible
-</t>
-        </is>
-      </c>
-      <c r="E41" t="inlineStr"/>
+          <t>$1552</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t> (9851 Harrison Rd, Bloomington Mn)</t>
+        </is>
+      </c>
       <c r="F41" t="inlineStr">
+        <is>
+          <t>2BR / 2Ba</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>1020ft2</t>
+        </is>
+      </c>
+      <c r="H41" t="inlineStr">
         <is>
           <t>
 QR Code Link to This Post
@@ -2843,28 +2933,30 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>
-2BR / 2.5Ba
-1515ft2
-available jul 5
-</t>
+          <t>https://minneapolis.craigslist.org/dak/apa/d/saint-paul-amazing-2-bedroom-townhome/6926087274.html</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>
-cats are OK - purrr
-dogs are OK - wooof
-townhouse
-w/d in unit
-no smoking
-attached garage
-wheelchair accessible
-</t>
-        </is>
-      </c>
-      <c r="E42" t="inlineStr"/>
+          <t>$1777</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t> (Apple Valley)</t>
+        </is>
+      </c>
       <c r="F42" t="inlineStr">
+        <is>
+          <t>2BR / 2.5Ba</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>1515ft2</t>
+        </is>
+      </c>
+      <c r="H42" t="inlineStr">
         <is>
           <t>
 QR Code Link to This Post
@@ -2916,28 +3008,30 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>
-3BR / 2Ba
-1475ft2
-available jul 5
-</t>
+          <t>https://minneapolis.craigslist.org/dak/apa/d/saint-paul-huge-3-bedroom-1475sqft/6926082248.html</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>
-cats are OK - purrr
-dogs are OK - wooof
-apartment
-w/d in unit
-no smoking
-attached garage
-wheelchair accessible
-</t>
-        </is>
-      </c>
-      <c r="E43" t="inlineStr"/>
+          <t>$2046</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t> (Apple Valley)</t>
+        </is>
+      </c>
       <c r="F43" t="inlineStr">
+        <is>
+          <t>3BR / 2Ba</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>1475ft2</t>
+        </is>
+      </c>
+      <c r="H43" t="inlineStr">
         <is>
           <t>
 QR Code Link to This Post
@@ -2985,27 +3079,30 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>
-2BR / 2Ba
-1082ft2
-</t>
+          <t>https://minneapolis.craigslist.org/hnp/apa/d/minneapolis-game-lounge-recycling-cafe/6925332193.html</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>
-cats are OK - purrr
-dogs are OK - wooof
-apartment
-w/d in unit
-no smoking
-attached garage
-wheelchair accessible
-</t>
-        </is>
-      </c>
-      <c r="E44" t="inlineStr"/>
+          <t>$2015</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>None Found</t>
+        </is>
+      </c>
       <c r="F44" t="inlineStr">
+        <is>
+          <t>2BR / 2Ba</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>1082ft2</t>
+        </is>
+      </c>
+      <c r="H44" t="inlineStr">
         <is>
           <t>
 QR Code Link to This Post
@@ -3044,27 +3141,30 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>
-2BR / 2Ba
-1193ft2
-</t>
+          <t>https://minneapolis.craigslist.org/hnp/apa/d/minneapolis-1000-discount-99-app-fee/6922499949.html</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>
-cats are OK - purrr
-dogs are OK - wooof
-apartment
-w/d in unit
-no smoking
-attached garage
-wheelchair accessible
-</t>
-        </is>
-      </c>
-      <c r="E45" t="inlineStr"/>
+          <t>$2125</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>None Found</t>
+        </is>
+      </c>
       <c r="F45" t="inlineStr">
+        <is>
+          <t>2BR / 2Ba</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>1193ft2</t>
+        </is>
+      </c>
+      <c r="H45" t="inlineStr">
         <is>
           <t>
 QR Code Link to This Post
@@ -3103,27 +3203,30 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>
-2BR / 2Ba
-1193ft2
-</t>
+          <t>https://minneapolis.craigslist.org/hnp/apa/d/minneapolis-elevator-walk-in-closet/6912110998.html</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>
-cats are OK - purrr
-dogs are OK - wooof
-apartment
-w/d in unit
-no smoking
-attached garage
-wheelchair accessible
-</t>
-        </is>
-      </c>
-      <c r="E46" t="inlineStr"/>
+          <t>$2125</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>None Found</t>
+        </is>
+      </c>
       <c r="F46" t="inlineStr">
+        <is>
+          <t>2BR / 2Ba</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>1193ft2</t>
+        </is>
+      </c>
+      <c r="H46" t="inlineStr">
         <is>
           <t>
 QR Code Link to This Post
@@ -3160,27 +3263,30 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>
-2BR / 2Ba
-1218ft2
-</t>
+          <t>https://minneapolis.craigslist.org/hnp/apa/d/minneapolis-co-working-zone-conference/6924742076.html</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>
-cats are OK - purrr
-dogs are OK - wooof
-apartment
-w/d in unit
-no smoking
-attached garage
-wheelchair accessible
-</t>
-        </is>
-      </c>
-      <c r="E47" t="inlineStr"/>
+          <t>$2260</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>None Found</t>
+        </is>
+      </c>
       <c r="F47" t="inlineStr">
+        <is>
+          <t>2BR / 2Ba</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>1218ft2</t>
+        </is>
+      </c>
+      <c r="H47" t="inlineStr">
         <is>
           <t>
 QR Code Link to This Post
@@ -3219,27 +3325,30 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>
-2BR / 2Ba
-1033ft2
-</t>
+          <t>https://minneapolis.craigslist.org/hnp/apa/d/minneapolis-the-lifestyle-you-deserve/6924663534.html</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>
-cats are OK - purrr
-dogs are OK - wooof
-apartment
-w/d in unit
-no smoking
-attached garage
-wheelchair accessible
-</t>
-        </is>
-      </c>
-      <c r="E48" t="inlineStr"/>
+          <t>$2360</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t> (7161 France Avenue South Edina, MN 55435)</t>
+        </is>
+      </c>
       <c r="F48" t="inlineStr">
+        <is>
+          <t>2BR / 2Ba</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>1033ft2</t>
+        </is>
+      </c>
+      <c r="H48" t="inlineStr">
         <is>
           <t>
 QR Code Link to This Post
@@ -3261,27 +3370,30 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>
-2BR / 2Ba
-992ft2
-</t>
+          <t>https://minneapolis.craigslist.org/hnp/apa/d/minneapolis-perfect-home-just-for-you/6924281745.html</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>
-cats are OK - purrr
-dogs are OK - wooof
-apartment
-w/d in unit
-no smoking
-attached garage
-wheelchair accessible
-</t>
-        </is>
-      </c>
-      <c r="E49" t="inlineStr"/>
+          <t>$2135</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t> (7161 France Avenue South Edina, MN 55435)</t>
+        </is>
+      </c>
       <c r="F49" t="inlineStr">
+        <is>
+          <t>2BR / 2Ba</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>992ft2</t>
+        </is>
+      </c>
+      <c r="H49" t="inlineStr">
         <is>
           <t>
 QR Code Link to This Post
@@ -3303,37 +3415,30 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>
-2BR / 2Ba
-1295ft2
-available sep 9
-</t>
+          <t>https://minneapolis.craigslist.org/hnp/apa/d/eden-prairie-spacious-2-bed-2-bath-top/6901858428.html</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>
-open house dates
-friday 2019-05-31
-saturday 2019-06-01
-sunday 2019-06-02
-</t>
+          <t>$1687</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>
-cats are OK - purrr
-dogs are OK - wooof
-apartment
-w/d in unit
-no smoking
-attached garage
-wheelchair accessible
-</t>
+          <t>None Found</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
+        <is>
+          <t>2BR / 2Ba</t>
+        </is>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>1295ft2</t>
+        </is>
+      </c>
+      <c r="H50" t="inlineStr">
         <is>
           <t>
 QR Code Link to This Post
@@ -3365,27 +3470,30 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>
-2BR / 2Ba
-1193ft2
-</t>
+          <t>https://minneapolis.craigslist.org/hnp/apa/d/minneapolis-smart-locks-fire-sprinklers/6920281397.html</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>
-cats are OK - purrr
-dogs are OK - wooof
-apartment
-w/d in unit
-no smoking
-attached garage
-wheelchair accessible
-</t>
-        </is>
-      </c>
-      <c r="E51" t="inlineStr"/>
+          <t>$2125</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>None Found</t>
+        </is>
+      </c>
       <c r="F51" t="inlineStr">
+        <is>
+          <t>2BR / 2Ba</t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>1193ft2</t>
+        </is>
+      </c>
+      <c r="H51" t="inlineStr">
         <is>
           <t>
 QR Code Link to This Post
@@ -3424,28 +3532,30 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>
-3BR / 2Ba
-1475ft2
-available jun 30
-</t>
+          <t>https://minneapolis.craigslist.org/dak/apa/d/saint-paul-huge-3-bedroom-ready-for/6921674009.html</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>
-cats are OK - purrr
-dogs are OK - wooof
-apartment
-w/d in unit
-no smoking
-attached garage
-wheelchair accessible
-</t>
-        </is>
-      </c>
-      <c r="E52" t="inlineStr"/>
+          <t>$2032</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t> (Apple Valley)</t>
+        </is>
+      </c>
       <c r="F52" t="inlineStr">
+        <is>
+          <t>3BR / 2Ba</t>
+        </is>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>1475ft2</t>
+        </is>
+      </c>
+      <c r="H52" t="inlineStr">
         <is>
           <t>
 QR Code Link to This Post
@@ -3493,27 +3603,30 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>
-2BR / 2Ba
-1193ft2
-</t>
+          <t>https://minneapolis.craigslist.org/hnp/apa/d/minneapolis-views-cafe-bike-storage/6915986106.html</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>
-cats are OK - purrr
-dogs are OK - wooof
-apartment
-w/d in unit
-no smoking
-attached garage
-wheelchair accessible
-</t>
-        </is>
-      </c>
-      <c r="E53" t="inlineStr"/>
+          <t>$2125</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>None Found</t>
+        </is>
+      </c>
       <c r="F53" t="inlineStr">
+        <is>
+          <t>2BR / 2Ba</t>
+        </is>
+      </c>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>1193ft2</t>
+        </is>
+      </c>
+      <c r="H53" t="inlineStr">
         <is>
           <t>
 QR Code Link to This Post
@@ -3550,27 +3663,30 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>
-2BR / 2Ba
-1082ft2
-</t>
+          <t>https://minneapolis.craigslist.org/hnp/apa/d/minneapolis-pet-friendly-media-room/6915153759.html</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>
-cats are OK - purrr
-dogs are OK - wooof
-apartment
-w/d in unit
-no smoking
-attached garage
-wheelchair accessible
-</t>
-        </is>
-      </c>
-      <c r="E54" t="inlineStr"/>
+          <t>$2005</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>None Found</t>
+        </is>
+      </c>
       <c r="F54" t="inlineStr">
+        <is>
+          <t>2BR / 2Ba</t>
+        </is>
+      </c>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>1082ft2</t>
+        </is>
+      </c>
+      <c r="H54" t="inlineStr">
         <is>
           <t>
 QR Code Link to This Post
@@ -3607,27 +3723,30 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>
-2BR / 2Ba
-1218ft2
-</t>
+          <t>https://minneapolis.craigslist.org/hnp/apa/d/minneapolis-cafe-clubhouse-recycling/6912214288.html</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>
-cats are OK - purrr
-dogs are OK - wooof
-apartment
-w/d in unit
-no smoking
-attached garage
-wheelchair accessible
-</t>
-        </is>
-      </c>
-      <c r="E55" t="inlineStr"/>
+          <t>$2260</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>None Found</t>
+        </is>
+      </c>
       <c r="F55" t="inlineStr">
+        <is>
+          <t>2BR / 2Ba</t>
+        </is>
+      </c>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t>1218ft2</t>
+        </is>
+      </c>
+      <c r="H55" t="inlineStr">
         <is>
           <t>
 QR Code Link to This Post
@@ -3664,27 +3783,30 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>
-2BR / 2Ba
-1218ft2
-</t>
+          <t>https://minneapolis.craigslist.org/hnp/apa/d/minneapolis-tile-backsplash-fire/6915750435.html</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>
-cats are OK - purrr
-dogs are OK - wooof
-apartment
-w/d in unit
-no smoking
-attached garage
-wheelchair accessible
-</t>
-        </is>
-      </c>
-      <c r="E56" t="inlineStr"/>
+          <t>$2260</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>None Found</t>
+        </is>
+      </c>
       <c r="F56" t="inlineStr">
+        <is>
+          <t>2BR / 2Ba</t>
+        </is>
+      </c>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t>1218ft2</t>
+        </is>
+      </c>
+      <c r="H56" t="inlineStr">
         <is>
           <t>
 QR Code Link to This Post
@@ -3721,28 +3843,30 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>
-3BR / 2Ba
-1444ft2
-available aug 2
-</t>
+          <t>https://minneapolis.craigslist.org/dak/apa/d/burnsville-beautiful-1st-floor-3/6917346634.html</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>
-cats are OK - purrr
-dogs are OK - wooof
-apartment
-w/d in unit
-no smoking
-attached garage
-wheelchair accessible
-</t>
-        </is>
-      </c>
-      <c r="E57" t="inlineStr"/>
+          <t>$1811</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t> (Lakeville MN)</t>
+        </is>
+      </c>
       <c r="F57" t="inlineStr">
+        <is>
+          <t>3BR / 2Ba</t>
+        </is>
+      </c>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t>1444ft2</t>
+        </is>
+      </c>
+      <c r="H57" t="inlineStr">
         <is>
           <t>
 QR Code Link to This Post
@@ -3778,28 +3902,30 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>
-3BR / 2Ba
-1475ft2
-available jun 21
-</t>
+          <t>https://minneapolis.craigslist.org/dak/apa/d/saint-paul-huge-3-bedroom-ready-for/6917194376.html</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>
-cats are OK - purrr
-dogs are OK - wooof
-apartment
-w/d in unit
-no smoking
-attached garage
-wheelchair accessible
-</t>
-        </is>
-      </c>
-      <c r="E58" t="inlineStr"/>
+          <t>$2032</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t> (Apple Valley)</t>
+        </is>
+      </c>
       <c r="F58" t="inlineStr">
+        <is>
+          <t>3BR / 2Ba</t>
+        </is>
+      </c>
+      <c r="G58" t="inlineStr">
+        <is>
+          <t>1475ft2</t>
+        </is>
+      </c>
+      <c r="H58" t="inlineStr">
         <is>
           <t>
 QR Code Link to This Post
@@ -3847,28 +3973,30 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>
-2BR / 2.5Ba
-1515ft2
-available jul 1
-</t>
+          <t>https://minneapolis.craigslist.org/dak/apa/d/saint-paul-amazing-2-bedroom-townhome/6916458683.html</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>
-cats are OK - purrr
-dogs are OK - wooof
-townhouse
-w/d in unit
-no smoking
-attached garage
-wheelchair accessible
-</t>
-        </is>
-      </c>
-      <c r="E59" t="inlineStr"/>
+          <t>$1720</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t> (Apple Valley)</t>
+        </is>
+      </c>
       <c r="F59" t="inlineStr">
+        <is>
+          <t>2BR / 2.5Ba</t>
+        </is>
+      </c>
+      <c r="G59" t="inlineStr">
+        <is>
+          <t>1515ft2</t>
+        </is>
+      </c>
+      <c r="H59" t="inlineStr">
         <is>
           <t>
 QR Code Link to This Post
@@ -3920,28 +4048,30 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>
-3BR / 2Ba
-1475ft2
-available jul 1
-</t>
+          <t>https://minneapolis.craigslist.org/dak/apa/d/saint-paul-huge-3-bedroom-ready-for/6916450536.html</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>
-cats are OK - purrr
-dogs are OK - wooof
-apartment
-w/d in unit
-no smoking
-attached garage
-wheelchair accessible
-</t>
-        </is>
-      </c>
-      <c r="E60" t="inlineStr"/>
+          <t>$2168</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t> (Apple Valley)</t>
+        </is>
+      </c>
       <c r="F60" t="inlineStr">
+        <is>
+          <t>3BR / 2Ba</t>
+        </is>
+      </c>
+      <c r="G60" t="inlineStr">
+        <is>
+          <t>1475ft2</t>
+        </is>
+      </c>
+      <c r="H60" t="inlineStr">
         <is>
           <t>
 QR Code Link to This Post
@@ -3988,27 +4118,30 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>
-2BR / 2Ba
-992ft2
-</t>
+          <t>https://minneapolis.craigslist.org/hnp/apa/d/minneapolis-best-view-of-edina-call-now/6914249893.html</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>
-cats are OK - purrr
-dogs are OK - wooof
-apartment
-w/d in unit
-no smoking
-attached garage
-wheelchair accessible
-</t>
-        </is>
-      </c>
-      <c r="E61" t="inlineStr"/>
+          <t>$2140</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>None Found</t>
+        </is>
+      </c>
       <c r="F61" t="inlineStr">
+        <is>
+          <t>2BR / 2Ba</t>
+        </is>
+      </c>
+      <c r="G61" t="inlineStr">
+        <is>
+          <t>992ft2</t>
+        </is>
+      </c>
+      <c r="H61" t="inlineStr">
         <is>
           <t>
 QR Code Link to This Post
@@ -4054,27 +4187,30 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>
-2BR / 2Ba
-1219ft2
-</t>
+          <t>https://minneapolis.craigslist.org/hnp/apa/d/minneapolis-recycling-fire-pits/6915883770.html</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>
-cats are OK - purrr
-dogs are OK - wooof
-apartment
-w/d in unit
-no smoking
-attached garage
-wheelchair accessible
-</t>
-        </is>
-      </c>
-      <c r="E62" t="inlineStr"/>
+          <t>$2145</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>None Found</t>
+        </is>
+      </c>
       <c r="F62" t="inlineStr">
+        <is>
+          <t>2BR / 2Ba</t>
+        </is>
+      </c>
+      <c r="G62" t="inlineStr">
+        <is>
+          <t>1219ft2</t>
+        </is>
+      </c>
+      <c r="H62" t="inlineStr">
         <is>
           <t>
 QR Code Link to This Post
@@ -4111,28 +4247,30 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>
-2BR / 2Ba
-1026ft2
-available aug 22
-</t>
+          <t>https://minneapolis.craigslist.org/hnp/apa/d/minneapolis-head-turning-style/6909130407.html</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>
-cats are OK - purrr
-dogs are OK - wooof
-apartment
-w/d in unit
-no smoking
-attached garage
-wheelchair accessible
-</t>
-        </is>
-      </c>
-      <c r="E63" t="inlineStr"/>
+          <t>$2370</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t> (7161 France Avenue South Edina, MN 55435)</t>
+        </is>
+      </c>
       <c r="F63" t="inlineStr">
+        <is>
+          <t>2BR / 2Ba</t>
+        </is>
+      </c>
+      <c r="G63" t="inlineStr">
+        <is>
+          <t>1026ft2</t>
+        </is>
+      </c>
+      <c r="H63" t="inlineStr">
         <is>
           <t>
 QR Code Link to This Post
@@ -4154,28 +4292,30 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>
-2BR / 2Ba
-992ft2
-available jun 5
-</t>
+          <t>https://minneapolis.craigslist.org/hnp/apa/d/minneapolis-at-last-this-is-what-youve/6900114257.html</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>
-cats are OK - purrr
-dogs are OK - wooof
-apartment
-w/d in unit
-no smoking
-attached garage
-wheelchair accessible
-</t>
-        </is>
-      </c>
-      <c r="E64" t="inlineStr"/>
+          <t>$2310</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t> (7161 France Avenue South Edina, MN 55435)</t>
+        </is>
+      </c>
       <c r="F64" t="inlineStr">
+        <is>
+          <t>2BR / 2Ba</t>
+        </is>
+      </c>
+      <c r="G64" t="inlineStr">
+        <is>
+          <t>992ft2</t>
+        </is>
+      </c>
+      <c r="H64" t="inlineStr">
         <is>
           <t>
 QR Code Link to This Post
@@ -4215,27 +4355,30 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>
-2BR / 2Ba
-1133ft2
-</t>
+          <t>https://minneapolis.craigslist.org/dak/apa/d/saint-paul-this-one-has-your-name-on-it/6914176875.html</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>
-cats are OK - purrr
-dogs are OK - wooof
-apartment
-w/d in unit
-no smoking
-attached garage
-wheelchair accessible
-</t>
-        </is>
-      </c>
-      <c r="E65" t="inlineStr"/>
+          <t>$1558</t>
+        </is>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t> (15464 Galaxie Avenue Apple Valley, MN)</t>
+        </is>
+      </c>
       <c r="F65" t="inlineStr">
+        <is>
+          <t>2BR / 2Ba</t>
+        </is>
+      </c>
+      <c r="G65" t="inlineStr">
+        <is>
+          <t>1133ft2</t>
+        </is>
+      </c>
+      <c r="H65" t="inlineStr">
         <is>
           <t>
 QR Code Link to This Post
@@ -4293,27 +4436,30 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>
-2BR / 2Ba
-1133ft2
-</t>
+          <t>https://minneapolis.craigslist.org/dak/apa/d/saint-paul-going-fast/6914170222.html</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>
-cats are OK - purrr
-dogs are OK - wooof
-apartment
-w/d in unit
-no smoking
-attached garage
-wheelchair accessible
-</t>
-        </is>
-      </c>
-      <c r="E66" t="inlineStr"/>
+          <t>$1558</t>
+        </is>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t> (15464 Galaxie Avenue Apple Valley, MN)</t>
+        </is>
+      </c>
       <c r="F66" t="inlineStr">
+        <is>
+          <t>2BR / 2Ba</t>
+        </is>
+      </c>
+      <c r="G66" t="inlineStr">
+        <is>
+          <t>1133ft2</t>
+        </is>
+      </c>
+      <c r="H66" t="inlineStr">
         <is>
           <t>
 QR Code Link to This Post
@@ -4371,27 +4517,30 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>
-2BR / 2Ba
-1133ft2
-</t>
+          <t>https://minneapolis.craigslist.org/dak/apa/d/saint-paul-get-it-before-its-gone/6914167269.html</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>
-cats are OK - purrr
-dogs are OK - wooof
-apartment
-w/d in unit
-no smoking
-attached garage
-wheelchair accessible
-</t>
-        </is>
-      </c>
-      <c r="E67" t="inlineStr"/>
+          <t>$1558</t>
+        </is>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t> (15464 Galaxie Avenue Apple Valley, MN)</t>
+        </is>
+      </c>
       <c r="F67" t="inlineStr">
+        <is>
+          <t>2BR / 2Ba</t>
+        </is>
+      </c>
+      <c r="G67" t="inlineStr">
+        <is>
+          <t>1133ft2</t>
+        </is>
+      </c>
+      <c r="H67" t="inlineStr">
         <is>
           <t>
 QR Code Link to This Post
@@ -4449,28 +4598,30 @@
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>
-2BR / 2Ba
-992ft2
-available jun 15
-</t>
+          <t>https://minneapolis.craigslist.org/hnp/apa/d/minneapolis-now-were-cooking-with-gas/6893470185.html</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>
-cats are OK - purrr
-dogs are OK - wooof
-apartment
-w/d in unit
-no smoking
-attached garage
-wheelchair accessible
-</t>
-        </is>
-      </c>
-      <c r="E68" t="inlineStr"/>
+          <t>$2265</t>
+        </is>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t> (7161 France Avenue South Edina, MN 55435)</t>
+        </is>
+      </c>
       <c r="F68" t="inlineStr">
+        <is>
+          <t>2BR / 2Ba</t>
+        </is>
+      </c>
+      <c r="G68" t="inlineStr">
+        <is>
+          <t>992ft2</t>
+        </is>
+      </c>
+      <c r="H68" t="inlineStr">
         <is>
           <t>
 QR Code Link to This Post

</xml_diff>